<commit_message>
video 1 parte 2
</commit_message>
<xml_diff>
--- a/src/main/java/Recursos/Data/Insumos/Testing.xlsx
+++ b/src/main/java/Recursos/Data/Insumos/Testing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\SeleniumJavaDesde0\src\main\java\Recursos\Data\Insumos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7375FBC-D86B-4B4A-9273-FF0673FF6D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2B5FB6-3BEE-43BF-8C05-871505FF3D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="26">
   <si>
     <t>usuario</t>
   </si>
@@ -94,12 +94,22 @@
   </si>
   <si>
     <t>jorge</t>
+  </si>
+  <si>
+    <t>fila</t>
+  </si>
+  <si>
+    <t>resultado</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -439,249 +449,291 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C7"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>25</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2">
+      <c r="H2" s="2">
         <v>1234</v>
       </c>
-      <c r="G2" s="2">
+      <c r="I2" s="2">
         <v>21</v>
       </c>
-      <c r="H2" s="2">
+      <c r="J2" s="2">
         <v>1997</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
+      <c r="B3" t="s" s="0">
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="2">
+      <c r="H3" s="2">
         <v>12345</v>
       </c>
-      <c r="G3" s="2">
+      <c r="I3" s="2">
         <v>26</v>
       </c>
-      <c r="H3" s="2">
+      <c r="J3" s="2">
         <v>1998</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="0">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="2">
+      <c r="H4" s="2">
         <v>1234</v>
       </c>
-      <c r="G4" s="2">
+      <c r="I4" s="2">
         <v>21</v>
       </c>
-      <c r="H4" s="2">
+      <c r="J4" s="2">
         <v>1997</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="0">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="2">
+      <c r="H5" s="2">
         <v>12345</v>
       </c>
-      <c r="G5" s="2">
+      <c r="I5" s="2">
         <v>26</v>
       </c>
-      <c r="H5" s="2">
+      <c r="J5" s="2">
         <v>1998</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="0">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="2">
+      <c r="H6" s="2">
         <v>1234</v>
       </c>
-      <c r="G6" s="2">
+      <c r="I6" s="2">
         <v>21</v>
       </c>
-      <c r="H6" s="2">
+      <c r="J6" s="2">
         <v>1997</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="0">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="2">
+      <c r="H7" s="2">
         <v>12345</v>
       </c>
-      <c r="G7" s="2">
+      <c r="I7" s="2">
         <v>26</v>
       </c>
-      <c r="H7" s="2">
+      <c r="J7" s="2">
         <v>1998</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>18</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{788DA741-3538-4E21-A683-8F5C7614803C}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{EFBA3E1A-7B84-407B-80A3-4B9499024FE1}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{6A9EC7FB-79FE-4C61-A334-BEC9D1C1BF49}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{2380D72D-6179-4521-84F0-709B05B1E3E9}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{213E7DF2-4DDD-4B3B-A248-3834437D26AD}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{C48B5656-2EBE-4999-9D56-F90531793ED3}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{788DA741-3538-4E21-A683-8F5C7614803C}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{EFBA3E1A-7B84-407B-80A3-4B9499024FE1}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{6A9EC7FB-79FE-4C61-A334-BEC9D1C1BF49}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{2380D72D-6179-4521-84F0-709B05B1E3E9}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{213E7DF2-4DDD-4B3B-A248-3834437D26AD}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{C48B5656-2EBE-4999-9D56-F90531793ED3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
se sube video 11_5
</commit_message>
<xml_diff>
--- a/src/main/java/Recursos/Data/Insumos/Testing.xlsx
+++ b/src/main/java/Recursos/Data/Insumos/Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\SeleniumJavaDesde0\src\main\java\Recursos\Data\Insumos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2B5FB6-3BEE-43BF-8C05-871505FF3D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72E92DB-9B1B-4130-889C-EE520FEE92E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7500" yWindow="5835" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="27">
   <si>
     <t>usuario</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>resultado</t>
+  </si>
+  <si>
+    <t>fallo</t>
   </si>
   <si>
     <t>ok</t>
@@ -452,15 +455,15 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.109375"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s" s="0">
         <v>23</v>
       </c>
@@ -498,12 +501,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="0">
         <v>1</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -536,12 +539,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="0">
         <v>2</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>2</v>
@@ -574,12 +577,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="0">
         <v>3</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>22</v>
@@ -612,12 +615,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="0">
         <v>4</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>19</v>
@@ -650,12 +653,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="0">
         <v>5</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>20</v>
@@ -688,12 +691,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="0">
         <v>6</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>21</v>

</xml_diff>